<commit_message>
Deploying to gh-pages from  @ 134f05946b1e3b7f57864be99ee2c0d46262f971 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/9.2.1.xlsx
+++ b/en/downloads/data-excel/9.2.1.xlsx
@@ -189,7 +189,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,12 +236,16 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -547,17 +551,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="37.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="36" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:17" ht="36" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -567,22 +573,23 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18"/>
-      <c r="O2" s="18"/>
+    <row r="2" spans="1:17" s="2" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
       <c r="P2" s="17"/>
+      <c r="Q2" s="21"/>
     </row>
-    <row r="3" spans="1:16" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -631,8 +638,11 @@
       <c r="P3" s="13">
         <v>2019</v>
       </c>
+      <c r="Q3" s="13">
+        <v>2020</v>
+      </c>
     </row>
-    <row r="4" spans="1:16" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -681,8 +691,11 @@
       <c r="P4" s="15">
         <v>14.7</v>
       </c>
+      <c r="Q4" s="19">
+        <v>14.5</v>
+      </c>
     </row>
-    <row r="5" spans="1:16" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" s="1" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -731,8 +744,11 @@
       <c r="P5" s="16">
         <v>14.7</v>
       </c>
+      <c r="Q5" s="16">
+        <v>13.8</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" s="2" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -740,20 +756,17 @@
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D2:O2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>